<commit_message>
:sparkles: Add r file for lab02
</commit_message>
<xml_diff>
--- a/lab02/grecja_ceny_stale_rebazowanie.xlsx
+++ b/lab02/grecja_ceny_stale_rebazowanie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\.vscode\extensions\studia\time_series\lab02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D86D152-1975-4556-91E3-34F0DA35DAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CFF32A-B5C3-459C-BAA9-A7A55C05A4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F48C9DC6-FF8C-47C1-9B73-2ECB170CCD0A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F48C9DC6-FF8C-47C1-9B73-2ECB170CCD0A}"/>
   </bookViews>
   <sheets>
     <sheet name="GVA Eurostat" sheetId="4" r:id="rId1"/>
@@ -53038,17 +53038,186 @@
     </row>
   </sheetData>
   <mergeCells count="203">
-    <mergeCell ref="OH10:OI10"/>
-    <mergeCell ref="OJ10:OK10"/>
-    <mergeCell ref="OL10:OM10"/>
-    <mergeCell ref="ON10:OO10"/>
-    <mergeCell ref="OP10:OQ10"/>
-    <mergeCell ref="NV10:NW10"/>
-    <mergeCell ref="NX10:NY10"/>
-    <mergeCell ref="NZ10:OA10"/>
-    <mergeCell ref="OB10:OC10"/>
-    <mergeCell ref="OD10:OE10"/>
-    <mergeCell ref="OF10:OG10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="AL10:AM10"/>
+    <mergeCell ref="AN10:AO10"/>
+    <mergeCell ref="AP10:AQ10"/>
+    <mergeCell ref="AR10:AS10"/>
+    <mergeCell ref="AT10:AU10"/>
+    <mergeCell ref="AV10:AW10"/>
+    <mergeCell ref="Z10:AA10"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="AF10:AG10"/>
+    <mergeCell ref="AH10:AI10"/>
+    <mergeCell ref="AJ10:AK10"/>
+    <mergeCell ref="BJ10:BK10"/>
+    <mergeCell ref="BL10:BM10"/>
+    <mergeCell ref="BN10:BO10"/>
+    <mergeCell ref="BP10:BQ10"/>
+    <mergeCell ref="BR10:BS10"/>
+    <mergeCell ref="BT10:BU10"/>
+    <mergeCell ref="AX10:AY10"/>
+    <mergeCell ref="AZ10:BA10"/>
+    <mergeCell ref="BB10:BC10"/>
+    <mergeCell ref="BD10:BE10"/>
+    <mergeCell ref="BF10:BG10"/>
+    <mergeCell ref="BH10:BI10"/>
+    <mergeCell ref="CH10:CI10"/>
+    <mergeCell ref="CJ10:CK10"/>
+    <mergeCell ref="CL10:CM10"/>
+    <mergeCell ref="CN10:CO10"/>
+    <mergeCell ref="CP10:CQ10"/>
+    <mergeCell ref="CR10:CS10"/>
+    <mergeCell ref="BV10:BW10"/>
+    <mergeCell ref="BX10:BY10"/>
+    <mergeCell ref="BZ10:CA10"/>
+    <mergeCell ref="CB10:CC10"/>
+    <mergeCell ref="CD10:CE10"/>
+    <mergeCell ref="CF10:CG10"/>
+    <mergeCell ref="DF10:DG10"/>
+    <mergeCell ref="DH10:DI10"/>
+    <mergeCell ref="DJ10:DK10"/>
+    <mergeCell ref="DL10:DM10"/>
+    <mergeCell ref="DN10:DO10"/>
+    <mergeCell ref="DP10:DQ10"/>
+    <mergeCell ref="CT10:CU10"/>
+    <mergeCell ref="CV10:CW10"/>
+    <mergeCell ref="CX10:CY10"/>
+    <mergeCell ref="CZ10:DA10"/>
+    <mergeCell ref="DB10:DC10"/>
+    <mergeCell ref="DD10:DE10"/>
+    <mergeCell ref="ED10:EE10"/>
+    <mergeCell ref="EF10:EG10"/>
+    <mergeCell ref="EH10:EI10"/>
+    <mergeCell ref="EJ10:EK10"/>
+    <mergeCell ref="EL10:EM10"/>
+    <mergeCell ref="EN10:EO10"/>
+    <mergeCell ref="DR10:DS10"/>
+    <mergeCell ref="DT10:DU10"/>
+    <mergeCell ref="DV10:DW10"/>
+    <mergeCell ref="DX10:DY10"/>
+    <mergeCell ref="DZ10:EA10"/>
+    <mergeCell ref="EB10:EC10"/>
+    <mergeCell ref="FB10:FC10"/>
+    <mergeCell ref="FD10:FE10"/>
+    <mergeCell ref="FF10:FG10"/>
+    <mergeCell ref="FH10:FI10"/>
+    <mergeCell ref="FJ10:FK10"/>
+    <mergeCell ref="FL10:FM10"/>
+    <mergeCell ref="EP10:EQ10"/>
+    <mergeCell ref="ER10:ES10"/>
+    <mergeCell ref="ET10:EU10"/>
+    <mergeCell ref="EV10:EW10"/>
+    <mergeCell ref="EX10:EY10"/>
+    <mergeCell ref="EZ10:FA10"/>
+    <mergeCell ref="FZ10:GA10"/>
+    <mergeCell ref="GB10:GC10"/>
+    <mergeCell ref="GD10:GE10"/>
+    <mergeCell ref="GF10:GG10"/>
+    <mergeCell ref="GH10:GI10"/>
+    <mergeCell ref="GJ10:GK10"/>
+    <mergeCell ref="FN10:FO10"/>
+    <mergeCell ref="FP10:FQ10"/>
+    <mergeCell ref="FR10:FS10"/>
+    <mergeCell ref="FT10:FU10"/>
+    <mergeCell ref="FV10:FW10"/>
+    <mergeCell ref="FX10:FY10"/>
+    <mergeCell ref="GX10:GY10"/>
+    <mergeCell ref="GZ10:HA10"/>
+    <mergeCell ref="HB10:HC10"/>
+    <mergeCell ref="HD10:HE10"/>
+    <mergeCell ref="HF10:HG10"/>
+    <mergeCell ref="HH10:HI10"/>
+    <mergeCell ref="GL10:GM10"/>
+    <mergeCell ref="GN10:GO10"/>
+    <mergeCell ref="GP10:GQ10"/>
+    <mergeCell ref="GR10:GS10"/>
+    <mergeCell ref="GT10:GU10"/>
+    <mergeCell ref="GV10:GW10"/>
+    <mergeCell ref="HV10:HW10"/>
+    <mergeCell ref="HX10:HY10"/>
+    <mergeCell ref="HZ10:IA10"/>
+    <mergeCell ref="IB10:IC10"/>
+    <mergeCell ref="ID10:IE10"/>
+    <mergeCell ref="IF10:IG10"/>
+    <mergeCell ref="HJ10:HK10"/>
+    <mergeCell ref="HL10:HM10"/>
+    <mergeCell ref="HN10:HO10"/>
+    <mergeCell ref="HP10:HQ10"/>
+    <mergeCell ref="HR10:HS10"/>
+    <mergeCell ref="HT10:HU10"/>
+    <mergeCell ref="IT10:IU10"/>
+    <mergeCell ref="IV10:IW10"/>
+    <mergeCell ref="IX10:IY10"/>
+    <mergeCell ref="IZ10:JA10"/>
+    <mergeCell ref="JB10:JC10"/>
+    <mergeCell ref="JD10:JE10"/>
+    <mergeCell ref="IH10:II10"/>
+    <mergeCell ref="IJ10:IK10"/>
+    <mergeCell ref="IL10:IM10"/>
+    <mergeCell ref="IN10:IO10"/>
+    <mergeCell ref="IP10:IQ10"/>
+    <mergeCell ref="IR10:IS10"/>
+    <mergeCell ref="JR10:JS10"/>
+    <mergeCell ref="JT10:JU10"/>
+    <mergeCell ref="JV10:JW10"/>
+    <mergeCell ref="JX10:JY10"/>
+    <mergeCell ref="JZ10:KA10"/>
+    <mergeCell ref="KB10:KC10"/>
+    <mergeCell ref="JF10:JG10"/>
+    <mergeCell ref="JH10:JI10"/>
+    <mergeCell ref="JJ10:JK10"/>
+    <mergeCell ref="JL10:JM10"/>
+    <mergeCell ref="JN10:JO10"/>
+    <mergeCell ref="JP10:JQ10"/>
+    <mergeCell ref="KP10:KQ10"/>
+    <mergeCell ref="KR10:KS10"/>
+    <mergeCell ref="KT10:KU10"/>
+    <mergeCell ref="KV10:KW10"/>
+    <mergeCell ref="KX10:KY10"/>
+    <mergeCell ref="KZ10:LA10"/>
+    <mergeCell ref="KD10:KE10"/>
+    <mergeCell ref="KF10:KG10"/>
+    <mergeCell ref="KH10:KI10"/>
+    <mergeCell ref="KJ10:KK10"/>
+    <mergeCell ref="KL10:KM10"/>
+    <mergeCell ref="KN10:KO10"/>
+    <mergeCell ref="LN10:LO10"/>
+    <mergeCell ref="LP10:LQ10"/>
+    <mergeCell ref="LR10:LS10"/>
+    <mergeCell ref="LT10:LU10"/>
+    <mergeCell ref="LV10:LW10"/>
+    <mergeCell ref="LX10:LY10"/>
+    <mergeCell ref="LB10:LC10"/>
+    <mergeCell ref="LD10:LE10"/>
+    <mergeCell ref="LF10:LG10"/>
+    <mergeCell ref="LH10:LI10"/>
+    <mergeCell ref="LJ10:LK10"/>
+    <mergeCell ref="LL10:LM10"/>
+    <mergeCell ref="ML10:MM10"/>
+    <mergeCell ref="MN10:MO10"/>
+    <mergeCell ref="MP10:MQ10"/>
+    <mergeCell ref="MR10:MS10"/>
+    <mergeCell ref="MT10:MU10"/>
+    <mergeCell ref="MV10:MW10"/>
+    <mergeCell ref="LZ10:MA10"/>
+    <mergeCell ref="MB10:MC10"/>
+    <mergeCell ref="MD10:ME10"/>
+    <mergeCell ref="MF10:MG10"/>
+    <mergeCell ref="MH10:MI10"/>
+    <mergeCell ref="MJ10:MK10"/>
     <mergeCell ref="NJ10:NK10"/>
     <mergeCell ref="NL10:NM10"/>
     <mergeCell ref="NN10:NO10"/>
@@ -53061,186 +53230,17 @@
     <mergeCell ref="ND10:NE10"/>
     <mergeCell ref="NF10:NG10"/>
     <mergeCell ref="NH10:NI10"/>
-    <mergeCell ref="ML10:MM10"/>
-    <mergeCell ref="MN10:MO10"/>
-    <mergeCell ref="MP10:MQ10"/>
-    <mergeCell ref="MR10:MS10"/>
-    <mergeCell ref="MT10:MU10"/>
-    <mergeCell ref="MV10:MW10"/>
-    <mergeCell ref="LZ10:MA10"/>
-    <mergeCell ref="MB10:MC10"/>
-    <mergeCell ref="MD10:ME10"/>
-    <mergeCell ref="MF10:MG10"/>
-    <mergeCell ref="MH10:MI10"/>
-    <mergeCell ref="MJ10:MK10"/>
-    <mergeCell ref="LN10:LO10"/>
-    <mergeCell ref="LP10:LQ10"/>
-    <mergeCell ref="LR10:LS10"/>
-    <mergeCell ref="LT10:LU10"/>
-    <mergeCell ref="LV10:LW10"/>
-    <mergeCell ref="LX10:LY10"/>
-    <mergeCell ref="LB10:LC10"/>
-    <mergeCell ref="LD10:LE10"/>
-    <mergeCell ref="LF10:LG10"/>
-    <mergeCell ref="LH10:LI10"/>
-    <mergeCell ref="LJ10:LK10"/>
-    <mergeCell ref="LL10:LM10"/>
-    <mergeCell ref="KP10:KQ10"/>
-    <mergeCell ref="KR10:KS10"/>
-    <mergeCell ref="KT10:KU10"/>
-    <mergeCell ref="KV10:KW10"/>
-    <mergeCell ref="KX10:KY10"/>
-    <mergeCell ref="KZ10:LA10"/>
-    <mergeCell ref="KD10:KE10"/>
-    <mergeCell ref="KF10:KG10"/>
-    <mergeCell ref="KH10:KI10"/>
-    <mergeCell ref="KJ10:KK10"/>
-    <mergeCell ref="KL10:KM10"/>
-    <mergeCell ref="KN10:KO10"/>
-    <mergeCell ref="JR10:JS10"/>
-    <mergeCell ref="JT10:JU10"/>
-    <mergeCell ref="JV10:JW10"/>
-    <mergeCell ref="JX10:JY10"/>
-    <mergeCell ref="JZ10:KA10"/>
-    <mergeCell ref="KB10:KC10"/>
-    <mergeCell ref="JF10:JG10"/>
-    <mergeCell ref="JH10:JI10"/>
-    <mergeCell ref="JJ10:JK10"/>
-    <mergeCell ref="JL10:JM10"/>
-    <mergeCell ref="JN10:JO10"/>
-    <mergeCell ref="JP10:JQ10"/>
-    <mergeCell ref="IT10:IU10"/>
-    <mergeCell ref="IV10:IW10"/>
-    <mergeCell ref="IX10:IY10"/>
-    <mergeCell ref="IZ10:JA10"/>
-    <mergeCell ref="JB10:JC10"/>
-    <mergeCell ref="JD10:JE10"/>
-    <mergeCell ref="IH10:II10"/>
-    <mergeCell ref="IJ10:IK10"/>
-    <mergeCell ref="IL10:IM10"/>
-    <mergeCell ref="IN10:IO10"/>
-    <mergeCell ref="IP10:IQ10"/>
-    <mergeCell ref="IR10:IS10"/>
-    <mergeCell ref="HV10:HW10"/>
-    <mergeCell ref="HX10:HY10"/>
-    <mergeCell ref="HZ10:IA10"/>
-    <mergeCell ref="IB10:IC10"/>
-    <mergeCell ref="ID10:IE10"/>
-    <mergeCell ref="IF10:IG10"/>
-    <mergeCell ref="HJ10:HK10"/>
-    <mergeCell ref="HL10:HM10"/>
-    <mergeCell ref="HN10:HO10"/>
-    <mergeCell ref="HP10:HQ10"/>
-    <mergeCell ref="HR10:HS10"/>
-    <mergeCell ref="HT10:HU10"/>
-    <mergeCell ref="GX10:GY10"/>
-    <mergeCell ref="GZ10:HA10"/>
-    <mergeCell ref="HB10:HC10"/>
-    <mergeCell ref="HD10:HE10"/>
-    <mergeCell ref="HF10:HG10"/>
-    <mergeCell ref="HH10:HI10"/>
-    <mergeCell ref="GL10:GM10"/>
-    <mergeCell ref="GN10:GO10"/>
-    <mergeCell ref="GP10:GQ10"/>
-    <mergeCell ref="GR10:GS10"/>
-    <mergeCell ref="GT10:GU10"/>
-    <mergeCell ref="GV10:GW10"/>
-    <mergeCell ref="FZ10:GA10"/>
-    <mergeCell ref="GB10:GC10"/>
-    <mergeCell ref="GD10:GE10"/>
-    <mergeCell ref="GF10:GG10"/>
-    <mergeCell ref="GH10:GI10"/>
-    <mergeCell ref="GJ10:GK10"/>
-    <mergeCell ref="FN10:FO10"/>
-    <mergeCell ref="FP10:FQ10"/>
-    <mergeCell ref="FR10:FS10"/>
-    <mergeCell ref="FT10:FU10"/>
-    <mergeCell ref="FV10:FW10"/>
-    <mergeCell ref="FX10:FY10"/>
-    <mergeCell ref="FB10:FC10"/>
-    <mergeCell ref="FD10:FE10"/>
-    <mergeCell ref="FF10:FG10"/>
-    <mergeCell ref="FH10:FI10"/>
-    <mergeCell ref="FJ10:FK10"/>
-    <mergeCell ref="FL10:FM10"/>
-    <mergeCell ref="EP10:EQ10"/>
-    <mergeCell ref="ER10:ES10"/>
-    <mergeCell ref="ET10:EU10"/>
-    <mergeCell ref="EV10:EW10"/>
-    <mergeCell ref="EX10:EY10"/>
-    <mergeCell ref="EZ10:FA10"/>
-    <mergeCell ref="ED10:EE10"/>
-    <mergeCell ref="EF10:EG10"/>
-    <mergeCell ref="EH10:EI10"/>
-    <mergeCell ref="EJ10:EK10"/>
-    <mergeCell ref="EL10:EM10"/>
-    <mergeCell ref="EN10:EO10"/>
-    <mergeCell ref="DR10:DS10"/>
-    <mergeCell ref="DT10:DU10"/>
-    <mergeCell ref="DV10:DW10"/>
-    <mergeCell ref="DX10:DY10"/>
-    <mergeCell ref="DZ10:EA10"/>
-    <mergeCell ref="EB10:EC10"/>
-    <mergeCell ref="DF10:DG10"/>
-    <mergeCell ref="DH10:DI10"/>
-    <mergeCell ref="DJ10:DK10"/>
-    <mergeCell ref="DL10:DM10"/>
-    <mergeCell ref="DN10:DO10"/>
-    <mergeCell ref="DP10:DQ10"/>
-    <mergeCell ref="CT10:CU10"/>
-    <mergeCell ref="CV10:CW10"/>
-    <mergeCell ref="CX10:CY10"/>
-    <mergeCell ref="CZ10:DA10"/>
-    <mergeCell ref="DB10:DC10"/>
-    <mergeCell ref="DD10:DE10"/>
-    <mergeCell ref="CH10:CI10"/>
-    <mergeCell ref="CJ10:CK10"/>
-    <mergeCell ref="CL10:CM10"/>
-    <mergeCell ref="CN10:CO10"/>
-    <mergeCell ref="CP10:CQ10"/>
-    <mergeCell ref="CR10:CS10"/>
-    <mergeCell ref="BV10:BW10"/>
-    <mergeCell ref="BX10:BY10"/>
-    <mergeCell ref="BZ10:CA10"/>
-    <mergeCell ref="CB10:CC10"/>
-    <mergeCell ref="CD10:CE10"/>
-    <mergeCell ref="CF10:CG10"/>
-    <mergeCell ref="BJ10:BK10"/>
-    <mergeCell ref="BL10:BM10"/>
-    <mergeCell ref="BN10:BO10"/>
-    <mergeCell ref="BP10:BQ10"/>
-    <mergeCell ref="BR10:BS10"/>
-    <mergeCell ref="BT10:BU10"/>
-    <mergeCell ref="AX10:AY10"/>
-    <mergeCell ref="AZ10:BA10"/>
-    <mergeCell ref="BB10:BC10"/>
-    <mergeCell ref="BD10:BE10"/>
-    <mergeCell ref="BF10:BG10"/>
-    <mergeCell ref="BH10:BI10"/>
-    <mergeCell ref="AL10:AM10"/>
-    <mergeCell ref="AN10:AO10"/>
-    <mergeCell ref="AP10:AQ10"/>
-    <mergeCell ref="AR10:AS10"/>
-    <mergeCell ref="AT10:AU10"/>
-    <mergeCell ref="AV10:AW10"/>
-    <mergeCell ref="Z10:AA10"/>
-    <mergeCell ref="AB10:AC10"/>
-    <mergeCell ref="AD10:AE10"/>
-    <mergeCell ref="AF10:AG10"/>
-    <mergeCell ref="AH10:AI10"/>
-    <mergeCell ref="AJ10:AK10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="T10:U10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:Y10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="OH10:OI10"/>
+    <mergeCell ref="OJ10:OK10"/>
+    <mergeCell ref="OL10:OM10"/>
+    <mergeCell ref="ON10:OO10"/>
+    <mergeCell ref="OP10:OQ10"/>
+    <mergeCell ref="NV10:NW10"/>
+    <mergeCell ref="NX10:NY10"/>
+    <mergeCell ref="NZ10:OA10"/>
+    <mergeCell ref="OB10:OC10"/>
+    <mergeCell ref="OD10:OE10"/>
+    <mergeCell ref="OF10:OG10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -53251,7 +53251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0271DA-F923-4983-9E1D-230678D0A36C}">
   <dimension ref="A1:T124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
@@ -57354,7 +57354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C73BF66-5B96-49CD-AAB6-27ECD3A5B762}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -58477,6 +58477,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="df20a811-f17a-454b-a878-f104ad76a41c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AA02DD375EACAC4FB15EEC8FD8FFC49B" ma:contentTypeVersion="15" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="d9297231a7b881470d0b5bd159be8dd9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df20a811-f17a-454b-a878-f104ad76a41c" xmlns:ns4="e4643e21-c9d5-45ab-a099-62e58f861c93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba0afb4d3d7e623bf79a49ad736390d0" ns3:_="" ns4:_="">
     <xsd:import namespace="df20a811-f17a-454b-a878-f104ad76a41c"/>
@@ -58711,38 +58728,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="df20a811-f17a-454b-a878-f104ad76a41c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD51091B-BF34-400C-B9FD-C73007A83DBC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E78EFEA6-9E00-44E6-BE4C-E0D8BB55713A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="df20a811-f17a-454b-a878-f104ad76a41c"/>
-    <ds:schemaRef ds:uri="e4643e21-c9d5-45ab-a099-62e58f861c93"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -58765,9 +58754,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E78EFEA6-9E00-44E6-BE4C-E0D8BB55713A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD51091B-BF34-400C-B9FD-C73007A83DBC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="df20a811-f17a-454b-a878-f104ad76a41c"/>
+    <ds:schemaRef ds:uri="e4643e21-c9d5-45ab-a099-62e58f861c93"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>